<commit_message>
able to update xlsx file with closed positions and refactored several methods for better readability
</commit_message>
<xml_diff>
--- a/trade_history.xlsx
+++ b/trade_history.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,13 +473,18 @@
           <t>exit</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>pnl</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>44721.05763700231</v>
+        <v>44730.03644305556</v>
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
@@ -493,16 +498,17 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>0.65156</v>
+        <v>0.46076</v>
       </c>
       <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>44721.0576571412</v>
+        <v>44730.03646423611</v>
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
@@ -512,43 +518,51 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
+          <t>short</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>3.331</v>
+      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>44730.0364677662</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>44730.04080313955</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>AVAX/USDT:USDT</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
           <t>long</t>
         </is>
       </c>
-      <c r="F3" t="n">
-        <v>5.822</v>
-      </c>
-      <c r="G3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="n">
-        <v>44721.05766150463</v>
-      </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>AVAX/USDT:USDT</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>long</t>
-        </is>
-      </c>
       <c r="F4" t="n">
-        <v>24.58</v>
-      </c>
-      <c r="G4" t="inlineStr"/>
+        <v>15.01</v>
+      </c>
+      <c r="G4" t="n">
+        <v>14.96</v>
+      </c>
+      <c r="H4" t="n">
+        <v>-0.3331112591605525</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>44721.05766486111</v>
+        <v>44730.03647100695</v>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
@@ -562,16 +576,17 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>30422</v>
+        <v>19285</v>
       </c>
       <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>44721.05766855324</v>
+        <v>44730.03647425926</v>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
@@ -585,18 +600,21 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>1809.3</v>
+        <v>1006.05</v>
       </c>
       <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>44721.05767168981</v>
-      </c>
-      <c r="C7" t="inlineStr"/>
+        <v>44730.0364772338</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>44730.03936880787</v>
+      </c>
       <c r="D7" t="inlineStr">
         <is>
           <t>FTM/USDT:USDT</t>
@@ -608,16 +626,21 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>0.3409</v>
-      </c>
-      <c r="G7" t="inlineStr"/>
+        <v>0.22</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.219</v>
+      </c>
+      <c r="H7" t="n">
+        <v>-0.454545454545455</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
+      <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>44721.05767506945</v>
+        <v>44730.03648079861</v>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
@@ -631,16 +654,17 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>39.371</v>
+        <v>28.599</v>
       </c>
       <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" t="n">
+      <c r="A9" s="1" t="n">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>44721.05767867673</v>
+        <v>44730.03649108797</v>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
@@ -654,9 +678,58 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>0.402</v>
+        <v>0.3091</v>
       </c>
       <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>44730.03936880787</v>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>FTM/USDT:USDT</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>short</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>0.219</v>
+      </c>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>44730.04080313657</v>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>AVAX/USDT:USDT</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>short</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>14.96</v>
+      </c>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>